<commit_message>
Documenta e finaliza projeto Paz Invest
Atualiza planilha, README e adiciona imagens do projeto
</commit_message>
<xml_diff>
--- a/Paz_Invest.xlsx
+++ b/Paz_Invest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Book\Documents\Análise de Dados - EBAC\Excel - Dio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Book\Documents\GitHub\Portfólio Dio\Dio---Excel-com-Intelig-ncia-Artificial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86504583-D98F-4F8F-8BC4-01022224FF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868DB3C4-10C9-4393-AFED-62EAD8611523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="0" xr2:uid="{E5ED4EA6-82B4-4864-AB74-5690EF6E2145}"/>
   </bookViews>
@@ -605,46 +605,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -654,27 +624,13 @@
     <xf numFmtId="10" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="8" fontId="9" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="8" fontId="9" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -693,16 +649,7 @@
     <xf numFmtId="164" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -750,6 +697,59 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2270,8 +2270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1846A83-B832-4F90-9880-3E984C5C7988}">
   <dimension ref="A11:M74"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36:D36"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A29" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2290,149 +2290,149 @@
   </cols>
   <sheetData>
     <row r="11" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="2:5" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8">
+      <c r="C12" s="63"/>
+      <c r="D12" s="5">
         <v>5000</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="2:5" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11">
+      <c r="C13" s="58"/>
+      <c r="D13" s="6">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="2:5" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14">
+      <c r="C14" s="61"/>
+      <c r="D14" s="7">
         <f>D12*30%</f>
         <v>1500</v>
       </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="2:5" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="58"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="39"/>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="2:5" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:13" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:13" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:13" ht="25.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
       <c r="E19" s="3"/>
       <c r="M19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="19">
+      <c r="C20" s="65"/>
+      <c r="D20" s="9">
         <v>500</v>
       </c>
       <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="20">
+      <c r="C21" s="58"/>
+      <c r="D21" s="10">
         <v>5</v>
       </c>
       <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="21">
+      <c r="C22" s="58"/>
+      <c r="D22" s="11">
         <v>1.0789999999999999E-2</v>
       </c>
       <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="24">
+      <c r="C23" s="69"/>
+      <c r="D23" s="12">
         <f>FV(taxa_mensal,quantidade_anos*12,aporte*-1)</f>
         <v>41888.456999243819</v>
       </c>
       <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="27">
+      <c r="C24" s="67"/>
+      <c r="D24" s="13">
         <f>patrimonio_acumulado*1%</f>
         <v>418.88456999243817</v>
       </c>
       <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B25" s="59"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="60"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="41"/>
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:13" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="28"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="14"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:13" ht="25.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="31" t="s">
+      <c r="C27" s="55"/>
+      <c r="D27" s="15" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2440,14 +2440,14 @@
       <c r="A28" s="1">
         <v>2</v>
       </c>
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="33">
+      <c r="C28" s="17">
         <f>FV(Planilha1!$D$22,Planilha1!A28*12,Planilha1!$D$20*-1)</f>
         <v>13613.813648822608</v>
       </c>
-      <c r="D28" s="34">
+      <c r="D28" s="18">
         <f>C28*rendimento_carteira</f>
         <v>122.52432283940347</v>
       </c>
@@ -2456,14 +2456,14 @@
       <c r="A29" s="1">
         <v>5</v>
       </c>
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="36">
+      <c r="C29" s="20">
         <f>FV(Planilha1!$D$22,Planilha1!A29*12,Planilha1!$D$20*-1)</f>
         <v>41888.456999243819</v>
       </c>
-      <c r="D29" s="37">
+      <c r="D29" s="21">
         <f>C29*rendimento_carteira</f>
         <v>376.99611299319434</v>
       </c>
@@ -2472,14 +2472,14 @@
       <c r="A30" s="1">
         <v>10</v>
       </c>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="36">
+      <c r="C30" s="20">
         <f>FV(Planilha1!$D$22,Planilha1!A30*12,Planilha1!$D$20*-1)</f>
         <v>121642.1062650861</v>
       </c>
-      <c r="D30" s="37">
+      <c r="D30" s="21">
         <f>C30*rendimento_carteira</f>
         <v>1094.7789563857748</v>
       </c>
@@ -2488,14 +2488,14 @@
       <c r="A31" s="1">
         <v>20</v>
       </c>
-      <c r="B31" s="35" t="s">
+      <c r="B31" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="36">
+      <c r="C31" s="20">
         <f>FV(Planilha1!$D$22,Planilha1!A31*12,Planilha1!$D$20*-1)</f>
         <v>562599.20004854025</v>
       </c>
-      <c r="D31" s="37">
+      <c r="D31" s="21">
         <f>C31*rendimento_carteira</f>
         <v>5063.3928004368618</v>
       </c>
@@ -2504,151 +2504,151 @@
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="39">
+      <c r="C32" s="23">
         <f>FV(Planilha1!$D$22,Planilha1!A32*12,Planilha1!$D$20*-1)</f>
         <v>2161084.8275023573</v>
       </c>
-      <c r="D32" s="40">
+      <c r="D32" s="24">
         <f>C32*rendimento_carteira</f>
         <v>19449.763447521214</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
-      <c r="B33" s="61"/>
-      <c r="C33" s="62"/>
-      <c r="D33" s="63"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="44"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B35" s="42" t="s">
+      <c r="B35" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="43" t="s">
+      <c r="C35" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="D35" s="43"/>
+      <c r="D35" s="53"/>
     </row>
     <row r="36" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B36" s="44" t="s">
+      <c r="B36" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="45">
+      <c r="C36" s="51">
         <f>aporte</f>
         <v>500</v>
       </c>
-      <c r="D36" s="46"/>
+      <c r="D36" s="52"/>
     </row>
     <row r="37" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="64"/>
-      <c r="C37" s="65"/>
-      <c r="D37" s="65"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
     </row>
     <row r="38" spans="1:4" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="41"/>
-      <c r="C38" s="41"/>
-      <c r="D38" s="41"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="47" t="s">
+      <c r="B39" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="47" t="s">
+      <c r="C39" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D39" s="47" t="s">
+      <c r="D39" s="28" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B40" s="48" t="s">
+      <c r="B40" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C40" s="66">
+      <c r="C40" s="47">
         <f>VLOOKUP($C$35&amp;"-"&amp;B40,Planilha2!$B:$E,4,FALSE)</f>
         <v>0.3</v>
       </c>
-      <c r="D40" s="69">
+      <c r="D40" s="50">
         <f>C40*$C$36</f>
         <v>150</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="48" t="s">
+      <c r="B41" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C41" s="66">
+      <c r="C41" s="47">
         <f>VLOOKUP($C$35&amp;"-"&amp;B41,Planilha2!$B:$E,4,FALSE)</f>
         <v>0.5</v>
       </c>
-      <c r="D41" s="69">
+      <c r="D41" s="50">
         <f t="shared" ref="D41:D45" si="0">C41*$C$36</f>
         <v>250</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B42" s="48" t="s">
+      <c r="B42" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C42" s="66">
+      <c r="C42" s="47">
         <f>VLOOKUP($C$35&amp;"-"&amp;B42,Planilha2!$B:$E,4,FALSE)</f>
         <v>0.1</v>
       </c>
-      <c r="D42" s="69">
+      <c r="D42" s="50">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B43" s="48" t="s">
+      <c r="B43" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="66">
+      <c r="C43" s="47">
         <f>VLOOKUP($C$35&amp;"-"&amp;B43,Planilha2!$B:$E,4,FALSE)</f>
         <v>0.1</v>
       </c>
-      <c r="D43" s="69">
+      <c r="D43" s="50">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B44" s="48" t="s">
+      <c r="B44" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C44" s="66">
+      <c r="C44" s="47">
         <f>VLOOKUP($C$35&amp;"-"&amp;B44,Planilha2!$B:$E,4,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="D44" s="69">
+      <c r="D44" s="50">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B45" s="48" t="s">
+      <c r="B45" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C45" s="66">
+      <c r="C45" s="47">
         <f>VLOOKUP($C$35&amp;"-"&amp;B45,Planilha2!$B:$E,4,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="D45" s="69">
+      <c r="D45" s="50">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B46" s="67"/>
-      <c r="C46" s="67"/>
-      <c r="D46" s="68">
+      <c r="B46" s="48"/>
+      <c r="C46" s="48"/>
+      <c r="D46" s="49">
         <f>SUM(D40:D45)</f>
         <v>500</v>
       </c>
@@ -2665,16 +2665,16 @@
     <row r="74" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B20:C20"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B20:C20"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B22:C22"/>
@@ -2708,19 +2708,19 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="47" t="s">
+      <c r="H3" s="28" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2732,16 +2732,16 @@
       <c r="C4" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="52">
+      <c r="E4" s="33">
         <v>0.3</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="51">
+      <c r="H4" s="32">
         <f>VLOOKUP(G4,$B:$E,4,FALSE)</f>
         <v>0.4</v>
       </c>
@@ -2754,10 +2754,10 @@
       <c r="C5" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="52">
+      <c r="E5" s="33">
         <v>0.5</v>
       </c>
     </row>
@@ -2769,10 +2769,10 @@
       <c r="C6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="52">
+      <c r="E6" s="33">
         <v>0.1</v>
       </c>
     </row>
@@ -2784,10 +2784,10 @@
       <c r="C7" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="52">
+      <c r="E7" s="33">
         <v>0.1</v>
       </c>
     </row>
@@ -2799,25 +2799,25 @@
       <c r="C8" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="52">
+      <c r="E8" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="49" t="str">
+      <c r="B9" s="30" t="str">
         <f t="shared" si="0"/>
         <v>Conservador-HOTELARIAS</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="50" t="s">
+      <c r="D9" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="53">
+      <c r="E9" s="34">
         <v>0</v>
       </c>
     </row>
@@ -2829,10 +2829,10 @@
       <c r="C10" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="48" t="s">
+      <c r="D10" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="54">
+      <c r="E10" s="35">
         <v>0.31</v>
       </c>
     </row>
@@ -2844,10 +2844,10 @@
       <c r="C11" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="48" t="s">
+      <c r="D11" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="54">
+      <c r="E11" s="35">
         <v>0.4</v>
       </c>
     </row>
@@ -2859,10 +2859,10 @@
       <c r="C12" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="48" t="s">
+      <c r="D12" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="54">
+      <c r="E12" s="35">
         <v>0.08</v>
       </c>
     </row>
@@ -2874,10 +2874,10 @@
       <c r="C13" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="48" t="s">
+      <c r="D13" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="54">
+      <c r="E13" s="35">
         <v>0.1</v>
       </c>
     </row>
@@ -2889,25 +2889,25 @@
       <c r="C14" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="48" t="s">
+      <c r="D14" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="54">
+      <c r="E14" s="35">
         <v>0.01</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="49" t="str">
+      <c r="B15" s="30" t="str">
         <f t="shared" si="0"/>
         <v>Moderado-HOTELARIAS</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="50" t="s">
+      <c r="D15" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="55">
+      <c r="E15" s="36">
         <v>0.1</v>
       </c>
     </row>
@@ -2919,10 +2919,10 @@
       <c r="C16" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="48" t="s">
+      <c r="D16" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="54">
+      <c r="E16" s="35">
         <v>0.5</v>
       </c>
     </row>
@@ -2934,10 +2934,10 @@
       <c r="C17" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="48" t="s">
+      <c r="D17" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="54">
+      <c r="E17" s="35">
         <v>0.1</v>
       </c>
     </row>
@@ -2949,10 +2949,10 @@
       <c r="C18" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="48" t="s">
+      <c r="D18" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="54">
+      <c r="E18" s="35">
         <v>0.05</v>
       </c>
     </row>
@@ -2964,10 +2964,10 @@
       <c r="C19" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="48" t="s">
+      <c r="D19" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="54">
+      <c r="E19" s="35">
         <v>0.05</v>
       </c>
     </row>
@@ -2979,10 +2979,10 @@
       <c r="C20" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="48" t="s">
+      <c r="D20" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="56">
+      <c r="E20" s="37">
         <v>0.2</v>
       </c>
     </row>
@@ -2994,10 +2994,10 @@
       <c r="C21" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="48" t="s">
+      <c r="D21" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="54">
+      <c r="E21" s="35">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>